<commit_message>
added more filters, fixed metrics
</commit_message>
<xml_diff>
--- a/data/multiple_donors.xlsx
+++ b/data/multiple_donors.xlsx
@@ -442,7 +442,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -487,12 +487,12 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">

</xml_diff>